<commit_message>
Changed figure labels and units
</commit_message>
<xml_diff>
--- a/data_input/Data_dictionary_2_Trait_thesaurus.xlsx
+++ b/data_input/Data_dictionary_2_Trait_thesaurus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sync\R Workspace\Zooplankton_trait_database\data_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5A7D937-A990-4DF6-94D5-A3EB7A182C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B663F2F-FC4A-411B-919D-A65331E969CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{55C0F0E5-0C6C-4754-B8D6-227AB5977D39}"/>
   </bookViews>
@@ -338,18 +338,12 @@
     <t>Weight-specific respiration rate as amount of oxygen consumed in an hour relative to the individual wet weight and standardized to 15°C.</t>
   </si>
   <si>
-    <t>excretion rate N</t>
-  </si>
-  <si>
     <t>excretionRateN_15C</t>
   </si>
   <si>
     <t>excretionRateN_WSDW_15C</t>
   </si>
   <si>
-    <t>excretion rate P</t>
-  </si>
-  <si>
     <t>excretionRateP_15C</t>
   </si>
   <si>
@@ -588,6 +582,12 @@
   </si>
   <si>
     <t>Trait bucket</t>
+  </si>
+  <si>
+    <t>excretion rate of ammonia</t>
+  </si>
+  <si>
+    <t>excretion rate of phosphate</t>
   </si>
 </sst>
 </file>
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93B72E8-FB11-4DE8-9520-BDB6B05A65F8}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -953,7 +953,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1432,7 +1432,7 @@
         <v>84</v>
       </c>
       <c r="D29" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E29" t="s">
         <v>85</v>
@@ -1449,7 +1449,7 @@
         <v>86</v>
       </c>
       <c r="D30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E30" t="s">
         <v>87</v>
@@ -1466,7 +1466,7 @@
         <v>88</v>
       </c>
       <c r="D31" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E31" t="s">
         <v>89</v>
@@ -1483,7 +1483,7 @@
         <v>92</v>
       </c>
       <c r="D32" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E32" t="s">
         <v>93</v>
@@ -1500,7 +1500,7 @@
         <v>94</v>
       </c>
       <c r="D33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E33" t="s">
         <v>95</v>
@@ -1517,7 +1517,7 @@
         <v>96</v>
       </c>
       <c r="D34" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E34" t="s">
         <v>97</v>
@@ -1534,7 +1534,7 @@
         <v>98</v>
       </c>
       <c r="D35" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E35" t="s">
         <v>99</v>
@@ -1545,16 +1545,16 @@
         <v>90</v>
       </c>
       <c r="B36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C36" t="s">
         <v>100</v>
       </c>
-      <c r="C36" t="s">
-        <v>101</v>
-      </c>
       <c r="D36" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E36" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.45">
@@ -1562,16 +1562,16 @@
         <v>90</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>182</v>
       </c>
       <c r="C37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D37" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E37" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.45">
@@ -1579,16 +1579,16 @@
         <v>90</v>
       </c>
       <c r="B38" t="s">
-        <v>103</v>
+        <v>183</v>
       </c>
       <c r="C38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D38" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E38" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.45">
@@ -1596,16 +1596,16 @@
         <v>90</v>
       </c>
       <c r="B39" t="s">
+        <v>183</v>
+      </c>
+      <c r="C39" t="s">
         <v>103</v>
       </c>
-      <c r="C39" t="s">
-        <v>105</v>
-      </c>
       <c r="D39" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E39" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.45">
@@ -1613,16 +1613,16 @@
         <v>90</v>
       </c>
       <c r="B40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40" t="s">
         <v>106</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" t="s">
         <v>107</v>
-      </c>
-      <c r="D40" t="s">
-        <v>108</v>
-      </c>
-      <c r="E40" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.45">
@@ -1630,264 +1630,264 @@
         <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C41" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" t="s">
+        <v>109</v>
+      </c>
+      <c r="E41" t="s">
         <v>110</v>
-      </c>
-      <c r="D41" t="s">
-        <v>111</v>
-      </c>
-      <c r="E41" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" t="s">
+        <v>112</v>
+      </c>
+      <c r="C42" t="s">
         <v>113</v>
       </c>
-      <c r="B42" t="s">
+      <c r="D42" t="s">
+        <v>175</v>
+      </c>
+      <c r="E42" t="s">
         <v>114</v>
-      </c>
-      <c r="C42" t="s">
-        <v>115</v>
-      </c>
-      <c r="D42" t="s">
-        <v>177</v>
-      </c>
-      <c r="E42" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D43" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E43" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B44" t="s">
+        <v>117</v>
+      </c>
+      <c r="C44" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" t="s">
+        <v>177</v>
+      </c>
+      <c r="E44" t="s">
         <v>119</v>
-      </c>
-      <c r="C44" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" t="s">
-        <v>179</v>
-      </c>
-      <c r="E44" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C45" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D45" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E45" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46" t="s">
+        <v>123</v>
+      </c>
+      <c r="E46" t="s">
         <v>124</v>
-      </c>
-      <c r="C46" t="s">
-        <v>125</v>
-      </c>
-      <c r="E46" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B47" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" t="s">
+        <v>126</v>
+      </c>
+      <c r="E47" t="s">
         <v>127</v>
-      </c>
-      <c r="C47" t="s">
-        <v>128</v>
-      </c>
-      <c r="E47" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" t="s">
+        <v>129</v>
+      </c>
+      <c r="E48" t="s">
         <v>130</v>
-      </c>
-      <c r="C48" t="s">
-        <v>131</v>
-      </c>
-      <c r="E48" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" t="s">
+        <v>132</v>
+      </c>
+      <c r="E49" t="s">
         <v>133</v>
-      </c>
-      <c r="C49" t="s">
-        <v>134</v>
-      </c>
-      <c r="E49" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B50" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" t="s">
+        <v>135</v>
+      </c>
+      <c r="E50" t="s">
         <v>136</v>
-      </c>
-      <c r="C50" t="s">
-        <v>137</v>
-      </c>
-      <c r="E50" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B51" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" t="s">
+        <v>138</v>
+      </c>
+      <c r="E51" t="s">
         <v>139</v>
-      </c>
-      <c r="C51" t="s">
-        <v>140</v>
-      </c>
-      <c r="E51" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
+        <v>140</v>
+      </c>
+      <c r="B52" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" t="s">
         <v>142</v>
       </c>
-      <c r="B52" t="s">
+      <c r="E52" t="s">
         <v>143</v>
-      </c>
-      <c r="C52" t="s">
-        <v>144</v>
-      </c>
-      <c r="E52" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B53" t="s">
+        <v>144</v>
+      </c>
+      <c r="C53" t="s">
+        <v>145</v>
+      </c>
+      <c r="D53" t="s">
         <v>146</v>
       </c>
-      <c r="C53" t="s">
+      <c r="E53" t="s">
         <v>147</v>
-      </c>
-      <c r="D53" t="s">
-        <v>148</v>
-      </c>
-      <c r="E53" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B54" t="s">
+        <v>148</v>
+      </c>
+      <c r="C54" t="s">
+        <v>149</v>
+      </c>
+      <c r="D54" t="s">
+        <v>179</v>
+      </c>
+      <c r="E54" t="s">
         <v>150</v>
-      </c>
-      <c r="C54" t="s">
-        <v>151</v>
-      </c>
-      <c r="D54" t="s">
-        <v>181</v>
-      </c>
-      <c r="E54" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B55" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C55" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D55" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E55" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B56" t="s">
+        <v>153</v>
+      </c>
+      <c r="C56" t="s">
+        <v>154</v>
+      </c>
+      <c r="D56" t="s">
         <v>155</v>
       </c>
-      <c r="C56" t="s">
+      <c r="E56" t="s">
         <v>156</v>
-      </c>
-      <c r="D56" t="s">
-        <v>157</v>
-      </c>
-      <c r="E56" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C57" t="s">
+        <v>157</v>
+      </c>
+      <c r="D57" t="s">
+        <v>158</v>
+      </c>
+      <c r="E57" t="s">
         <v>159</v>
-      </c>
-      <c r="D57" t="s">
-        <v>160</v>
-      </c>
-      <c r="E57" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>